<commit_message>
FInxed column name 'Hora inicio'
</commit_message>
<xml_diff>
--- a/241204_costes.xlsx
+++ b/241204_costes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20415"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\miguel OneDrive\OneDrive - Universidad Politécnica de Madrid\docencia_24_25\mca_2425\entregas\Entrega 3 - Generacion columnas\datos quirófanos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Feder\Desktop\GitHub\entrega-3-gc-grupo-mca-o\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="11_AD4D2F04E46CFB4ACB3E206EE515CB30683EDF16" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{B1B7C383-A30F-41BA-B83E-302B67C9B396}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EBB6906-A452-498F-9139-3C66639CA563}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="costes" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,17 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -921,7 +932,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1199,120 +1210,120 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:FT100"/>
+  <dimension ref="A1:FT102"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="K102" sqref="K102"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.54296875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="15.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="15.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="15.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="14.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="18" width="14.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="14.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="23" max="25" width="14.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="26" max="27" width="15.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="28" max="29" width="14.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="31" max="32" width="14.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="15.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="13.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="35" max="40" width="14.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="41" max="43" width="15.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="14.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="15.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="14.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="15.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="14.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="49" max="53" width="15.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="54" max="56" width="14.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="15.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="58" max="59" width="14.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="15.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="14.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="15.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="63" max="65" width="14.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="15.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="67" max="69" width="14.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="15.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="14.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="13.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="14.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="15.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="13.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="14.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="13.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="14.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="79" max="83" width="15.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="14.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="15.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="86" max="87" width="14.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="15.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="89" max="92" width="14.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="93" max="94" width="15.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="95" max="96" width="14.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="97" max="98" width="15.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="99" max="104" width="14.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="105" max="105" width="15.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="106" max="110" width="14.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="111" max="111" width="15.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="112" max="113" width="14.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="114" max="114" width="15.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="115" max="115" width="14.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="116" max="118" width="15.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="119" max="119" width="14.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="120" max="121" width="15.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="122" max="125" width="14.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="126" max="127" width="15.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="128" max="129" width="14.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="130" max="130" width="15.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="131" max="131" width="13.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="132" max="132" width="15.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="133" max="133" width="14.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="134" max="139" width="15.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="140" max="140" width="13.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="141" max="143" width="15.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="144" max="144" width="14.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="145" max="145" width="15.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="146" max="146" width="14.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="147" max="147" width="15.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="148" max="148" width="13.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="149" max="149" width="15.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="150" max="150" width="14.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="151" max="151" width="15.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="152" max="152" width="14.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="153" max="154" width="13.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="155" max="156" width="14.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="157" max="158" width="15.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="159" max="161" width="14.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="162" max="162" width="15.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="163" max="163" width="14.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="164" max="164" width="15.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="165" max="166" width="14.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="167" max="167" width="15.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="168" max="168" width="16.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="169" max="169" width="15.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="170" max="171" width="14.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="172" max="172" width="15.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="173" max="173" width="14.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="174" max="174" width="15.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="175" max="175" width="14.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="176" max="176" width="15.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="177" max="16384" width="9.1796875" style="3"/>
+    <col min="1" max="1" width="16.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="15.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="15.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="15.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="14.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="14.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="14.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="23" max="25" width="14.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="26" max="27" width="15.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="14.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="31" max="32" width="14.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="15.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="13.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="35" max="40" width="14.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="41" max="43" width="15.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="14.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="15.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="14.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="15.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="14.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="49" max="53" width="15.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="54" max="56" width="14.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="15.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="58" max="59" width="14.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="15.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="14.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="15.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="63" max="65" width="14.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="15.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="67" max="69" width="14.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="15.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="14.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="13.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="14.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="15.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="13.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="14.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="13.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="14.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="79" max="83" width="15.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="14.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="15.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="86" max="87" width="14.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="15.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="89" max="92" width="14.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="93" max="94" width="15.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="95" max="96" width="14.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="97" max="98" width="15.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="99" max="104" width="14.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="105" max="105" width="15.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="106" max="110" width="14.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="111" max="111" width="15.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="112" max="113" width="14.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="114" max="114" width="15.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="115" max="115" width="14.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="116" max="118" width="15.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="119" max="119" width="14.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="120" max="121" width="15.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="122" max="125" width="14.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="126" max="127" width="15.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="128" max="129" width="14.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="130" max="130" width="15.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="131" max="131" width="13.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="132" max="132" width="15.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="133" max="133" width="14.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="134" max="139" width="15.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="140" max="140" width="13.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="141" max="143" width="15.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="144" max="144" width="14.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="145" max="145" width="15.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="146" max="146" width="14.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="147" max="147" width="15.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="148" max="148" width="13.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="149" max="149" width="15.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="150" max="150" width="14.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="151" max="151" width="15.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="152" max="152" width="14.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="153" max="154" width="13.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="155" max="156" width="14.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="157" max="158" width="15.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="159" max="161" width="14.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="162" max="162" width="15.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="163" max="163" width="14.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="164" max="164" width="15.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="165" max="166" width="14.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="167" max="167" width="15.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="168" max="168" width="16.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="169" max="169" width="15.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="170" max="171" width="14.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="172" max="172" width="15.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="173" max="173" width="14.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="174" max="174" width="15.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="175" max="175" width="14.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="176" max="176" width="15.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="177" max="16384" width="9.21875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:176" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:176" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1840,7 +1851,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="2" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>175</v>
       </c>
@@ -2370,7 +2381,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="3" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>176</v>
       </c>
@@ -2900,7 +2911,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="4" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>177</v>
       </c>
@@ -3430,7 +3441,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="5" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>178</v>
       </c>
@@ -3960,7 +3971,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="6" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>179</v>
       </c>
@@ -4490,7 +4501,7 @@
         <v>869</v>
       </c>
     </row>
-    <row r="7" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>180</v>
       </c>
@@ -5020,7 +5031,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="8" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>181</v>
       </c>
@@ -5550,7 +5561,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="9" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>182</v>
       </c>
@@ -6080,7 +6091,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="10" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>183</v>
       </c>
@@ -6610,7 +6621,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="11" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>184</v>
       </c>
@@ -7140,7 +7151,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="12" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>185</v>
       </c>
@@ -7670,7 +7681,7 @@
         <v>857</v>
       </c>
     </row>
-    <row r="13" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>186</v>
       </c>
@@ -8200,7 +8211,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="14" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>187</v>
       </c>
@@ -8730,7 +8741,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="15" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>188</v>
       </c>
@@ -9260,7 +9271,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="16" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>189</v>
       </c>
@@ -9790,7 +9801,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="17" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>190</v>
       </c>
@@ -10320,7 +10331,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="18" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>191</v>
       </c>
@@ -10850,7 +10861,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="19" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>192</v>
       </c>
@@ -11380,7 +11391,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="20" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>193</v>
       </c>
@@ -11910,7 +11921,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="21" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>194</v>
       </c>
@@ -12440,7 +12451,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="22" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>195</v>
       </c>
@@ -12970,7 +12981,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="23" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>196</v>
       </c>
@@ -13500,7 +13511,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="24" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>197</v>
       </c>
@@ -14030,7 +14041,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="25" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>198</v>
       </c>
@@ -14560,7 +14571,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="26" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>199</v>
       </c>
@@ -15090,7 +15101,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="27" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>200</v>
       </c>
@@ -15620,7 +15631,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="28" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>201</v>
       </c>
@@ -16150,7 +16161,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="29" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>202</v>
       </c>
@@ -16680,7 +16691,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="30" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>203</v>
       </c>
@@ -17210,7 +17221,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="31" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>204</v>
       </c>
@@ -17740,7 +17751,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="32" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>205</v>
       </c>
@@ -18270,7 +18281,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="33" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>206</v>
       </c>
@@ -18800,7 +18811,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="34" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>207</v>
       </c>
@@ -19330,7 +19341,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="35" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>208</v>
       </c>
@@ -19860,7 +19871,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="36" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>209</v>
       </c>
@@ -20390,7 +20401,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="37" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>210</v>
       </c>
@@ -20920,7 +20931,7 @@
         <v>793</v>
       </c>
     </row>
-    <row r="38" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>211</v>
       </c>
@@ -21450,7 +21461,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="39" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>212</v>
       </c>
@@ -21980,7 +21991,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="40" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>213</v>
       </c>
@@ -22510,7 +22521,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="41" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>214</v>
       </c>
@@ -23040,7 +23051,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="42" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>215</v>
       </c>
@@ -23570,7 +23581,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="43" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>216</v>
       </c>
@@ -24100,7 +24111,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="44" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>217</v>
       </c>
@@ -24630,7 +24641,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="45" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>218</v>
       </c>
@@ -25160,7 +25171,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="46" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>219</v>
       </c>
@@ -25690,7 +25701,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="47" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>220</v>
       </c>
@@ -26220,7 +26231,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="48" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>221</v>
       </c>
@@ -26750,7 +26761,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="49" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>222</v>
       </c>
@@ -27280,7 +27291,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="50" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>223</v>
       </c>
@@ -27810,7 +27821,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="51" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>224</v>
       </c>
@@ -28340,7 +28351,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="52" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>225</v>
       </c>
@@ -28870,7 +28881,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="53" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>226</v>
       </c>
@@ -29400,7 +29411,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="54" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>227</v>
       </c>
@@ -29930,7 +29941,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="55" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>228</v>
       </c>
@@ -30460,7 +30471,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="56" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>229</v>
       </c>
@@ -30990,7 +31001,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="57" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>230</v>
       </c>
@@ -31520,7 +31531,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="58" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>231</v>
       </c>
@@ -32050,7 +32061,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="59" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>232</v>
       </c>
@@ -32580,7 +32591,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="60" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>233</v>
       </c>
@@ -33110,7 +33121,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="61" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>234</v>
       </c>
@@ -33640,7 +33651,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="62" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>235</v>
       </c>
@@ -34170,7 +34181,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="63" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>236</v>
       </c>
@@ -34700,7 +34711,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="64" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>237</v>
       </c>
@@ -35230,7 +35241,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="65" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>238</v>
       </c>
@@ -35760,7 +35771,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="66" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>239</v>
       </c>
@@ -36290,7 +36301,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="67" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>240</v>
       </c>
@@ -36820,7 +36831,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="68" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>241</v>
       </c>
@@ -37350,7 +37361,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="69" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>242</v>
       </c>
@@ -37880,7 +37891,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="70" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>243</v>
       </c>
@@ -38410,7 +38421,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="71" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>244</v>
       </c>
@@ -38940,7 +38951,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="72" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>245</v>
       </c>
@@ -39470,7 +39481,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="73" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>246</v>
       </c>
@@ -40000,7 +40011,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="74" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>247</v>
       </c>
@@ -40530,7 +40541,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="75" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>248</v>
       </c>
@@ -41060,7 +41071,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="76" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>249</v>
       </c>
@@ -41590,7 +41601,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="77" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>250</v>
       </c>
@@ -42120,7 +42131,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="78" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>251</v>
       </c>
@@ -42650,7 +42661,7 @@
         <v>844</v>
       </c>
     </row>
-    <row r="79" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>252</v>
       </c>
@@ -43180,7 +43191,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="80" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>253</v>
       </c>
@@ -43710,7 +43721,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="81" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>254</v>
       </c>
@@ -44240,7 +44251,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="82" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>255</v>
       </c>
@@ -44770,7 +44781,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="83" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>256</v>
       </c>
@@ -45300,7 +45311,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="84" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>257</v>
       </c>
@@ -45830,7 +45841,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="85" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>258</v>
       </c>
@@ -46360,7 +46371,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="86" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>259</v>
       </c>
@@ -46890,7 +46901,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="87" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>260</v>
       </c>
@@ -47420,7 +47431,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="88" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>261</v>
       </c>
@@ -47950,7 +47961,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="89" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>262</v>
       </c>
@@ -48480,7 +48491,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="90" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>263</v>
       </c>
@@ -49010,7 +49021,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="91" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>264</v>
       </c>
@@ -49540,7 +49551,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="92" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>265</v>
       </c>
@@ -50070,7 +50081,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="93" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>266</v>
       </c>
@@ -50600,7 +50611,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="94" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>267</v>
       </c>
@@ -51130,7 +51141,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="95" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
         <v>268</v>
       </c>
@@ -51660,7 +51671,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="96" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>269</v>
       </c>
@@ -52190,7 +52201,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="97" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>270</v>
       </c>
@@ -52720,7 +52731,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="98" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>271</v>
       </c>
@@ -53250,7 +53261,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="99" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>272</v>
       </c>
@@ -53780,7 +53791,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="100" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:176" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
         <v>273</v>
       </c>
@@ -54308,6 +54319,12 @@
       </c>
       <c r="FT100" s="2">
         <v>451</v>
+      </c>
+    </row>
+    <row r="102" spans="1:176" x14ac:dyDescent="0.3">
+      <c r="K102" s="3">
+        <f>AVERAGE(K2:K100)</f>
+        <v>488.88888888888891</v>
       </c>
     </row>
   </sheetData>

</xml_diff>